<commit_message>
3ra semana 2 ciclo
</commit_message>
<xml_diff>
--- a/DATA/Asistencias.xlsx
+++ b/DATA/Asistencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdelc\Desktop\Asistencia\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C63793-9270-463E-AE51-260A5D69BB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7672DBB-E167-48BF-B26E-C460A6EA99EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,7 +602,7 @@
   <dimension ref="A1:D571"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D350" sqref="D350"/>
+      <selection activeCell="D578" sqref="D578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6154,7 +6154,7 @@
         <v>3</v>
       </c>
       <c r="D396" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.3">
@@ -6168,7 +6168,7 @@
         <v>3</v>
       </c>
       <c r="D397" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.3">
@@ -6238,7 +6238,7 @@
         <v>3</v>
       </c>
       <c r="D402" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.3">
@@ -6294,7 +6294,7 @@
         <v>3</v>
       </c>
       <c r="D406" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.3">
@@ -6308,7 +6308,7 @@
         <v>3</v>
       </c>
       <c r="D407" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.3">
@@ -6336,7 +6336,7 @@
         <v>3</v>
       </c>
       <c r="D409" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.3">
@@ -6420,7 +6420,7 @@
         <v>3</v>
       </c>
       <c r="D415" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.3">
@@ -6490,7 +6490,7 @@
         <v>3</v>
       </c>
       <c r="D420" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.3">
@@ -6504,7 +6504,7 @@
         <v>3</v>
       </c>
       <c r="D421" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.3">
@@ -6518,7 +6518,7 @@
         <v>3</v>
       </c>
       <c r="D422" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.3">
@@ -6532,7 +6532,7 @@
         <v>3</v>
       </c>
       <c r="D423" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.3">
@@ -6546,7 +6546,7 @@
         <v>3</v>
       </c>
       <c r="D424" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.3">
@@ -6560,7 +6560,7 @@
         <v>3</v>
       </c>
       <c r="D425" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.3">
@@ -6574,7 +6574,7 @@
         <v>3</v>
       </c>
       <c r="D426" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.3">
@@ -6588,7 +6588,7 @@
         <v>3</v>
       </c>
       <c r="D427" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.3">
@@ -6602,7 +6602,7 @@
         <v>3</v>
       </c>
       <c r="D428" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
@@ -6616,7 +6616,7 @@
         <v>3</v>
       </c>
       <c r="D429" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.3">
@@ -6630,7 +6630,7 @@
         <v>3</v>
       </c>
       <c r="D430" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.3">
@@ -6644,7 +6644,7 @@
         <v>3</v>
       </c>
       <c r="D431" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.3">
@@ -6658,7 +6658,7 @@
         <v>3</v>
       </c>
       <c r="D432" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.3">
@@ -6672,7 +6672,7 @@
         <v>3</v>
       </c>
       <c r="D433" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.3">
@@ -6714,7 +6714,7 @@
         <v>3</v>
       </c>
       <c r="D436" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.3">
@@ -6728,7 +6728,7 @@
         <v>3</v>
       </c>
       <c r="D437" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.3">
@@ -6742,7 +6742,7 @@
         <v>3</v>
       </c>
       <c r="D438" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.3">
@@ -6756,7 +6756,7 @@
         <v>3</v>
       </c>
       <c r="D439" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.3">
@@ -6798,7 +6798,7 @@
         <v>3</v>
       </c>
       <c r="D442" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.3">
@@ -6812,7 +6812,7 @@
         <v>3</v>
       </c>
       <c r="D443" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.3">
@@ -6826,7 +6826,7 @@
         <v>3</v>
       </c>
       <c r="D444" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.3">
@@ -6840,7 +6840,7 @@
         <v>3</v>
       </c>
       <c r="D445" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.3">
@@ -6938,7 +6938,7 @@
         <v>3</v>
       </c>
       <c r="D452" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
4 semana del 2 ciclo
</commit_message>
<xml_diff>
--- a/DATA/Asistencias.xlsx
+++ b/DATA/Asistencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdelc\Desktop\Asistencia\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7672DBB-E167-48BF-B26E-C460A6EA99EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57235756-78EA-4939-A1B5-48B8F297BF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,7 +602,7 @@
   <dimension ref="A1:D571"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D578" sqref="D578"/>
+      <selection activeCell="D291" sqref="D291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +750,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1534,7 +1534,7 @@
         <v>2</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1548,7 +1548,7 @@
         <v>2</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2318,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2332,7 +2332,7 @@
         <v>3</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3102,7 +3102,7 @@
         <v>4</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3116,7 +3116,7 @@
         <v>4</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5356,7 +5356,7 @@
         <v>2</v>
       </c>
       <c r="D339" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.3">
@@ -5412,7 +5412,7 @@
         <v>2</v>
       </c>
       <c r="D343" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.3">
@@ -5426,7 +5426,7 @@
         <v>2</v>
       </c>
       <c r="D344" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.3">
@@ -5440,7 +5440,7 @@
         <v>2</v>
       </c>
       <c r="D345" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.3">
@@ -5454,7 +5454,7 @@
         <v>2</v>
       </c>
       <c r="D346" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.3">
@@ -5468,7 +5468,7 @@
         <v>2</v>
       </c>
       <c r="D347" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.3">
@@ -5482,7 +5482,7 @@
         <v>2</v>
       </c>
       <c r="D348" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.3">
@@ -5524,7 +5524,7 @@
         <v>2</v>
       </c>
       <c r="D351" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.3">
@@ -5580,7 +5580,7 @@
         <v>2</v>
       </c>
       <c r="D355" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.3">
@@ -5594,7 +5594,7 @@
         <v>2</v>
       </c>
       <c r="D356" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.3">
@@ -5832,7 +5832,7 @@
         <v>2</v>
       </c>
       <c r="D373" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.3">
@@ -5846,7 +5846,7 @@
         <v>2</v>
       </c>
       <c r="D374" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.3">
@@ -5888,7 +5888,7 @@
         <v>2</v>
       </c>
       <c r="D377" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.3">
@@ -5902,7 +5902,7 @@
         <v>2</v>
       </c>
       <c r="D378" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.3">
@@ -5916,7 +5916,7 @@
         <v>2</v>
       </c>
       <c r="D379" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.3">
@@ -5930,7 +5930,7 @@
         <v>2</v>
       </c>
       <c r="D380" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.3">
@@ -5972,7 +5972,7 @@
         <v>2</v>
       </c>
       <c r="D383" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.3">
@@ -5986,7 +5986,7 @@
         <v>2</v>
       </c>
       <c r="D384" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.3">
@@ -6056,7 +6056,7 @@
         <v>2</v>
       </c>
       <c r="D389" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.3">
@@ -6070,7 +6070,7 @@
         <v>2</v>
       </c>
       <c r="D390" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.3">
@@ -6084,7 +6084,7 @@
         <v>2</v>
       </c>
       <c r="D391" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.3">
@@ -6098,7 +6098,7 @@
         <v>2</v>
       </c>
       <c r="D392" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.3">
@@ -6112,7 +6112,7 @@
         <v>2</v>
       </c>
       <c r="D393" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.3">
@@ -6126,7 +6126,7 @@
         <v>2</v>
       </c>
       <c r="D394" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.3">
@@ -6182,7 +6182,7 @@
         <v>3</v>
       </c>
       <c r="D398" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
@@ -6196,7 +6196,7 @@
         <v>3</v>
       </c>
       <c r="D399" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.3">
@@ -6210,7 +6210,7 @@
         <v>3</v>
       </c>
       <c r="D400" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.3">
@@ -6224,7 +6224,7 @@
         <v>3</v>
       </c>
       <c r="D401" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.3">
@@ -6252,7 +6252,7 @@
         <v>3</v>
       </c>
       <c r="D403" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.3">
@@ -6266,7 +6266,7 @@
         <v>3</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.3">
@@ -6280,7 +6280,7 @@
         <v>3</v>
       </c>
       <c r="D405" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.3">
@@ -6322,7 +6322,7 @@
         <v>3</v>
       </c>
       <c r="D408" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.3">
@@ -6350,7 +6350,7 @@
         <v>3</v>
       </c>
       <c r="D410" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.3">
@@ -6364,7 +6364,7 @@
         <v>3</v>
       </c>
       <c r="D411" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.3">
@@ -6378,7 +6378,7 @@
         <v>3</v>
       </c>
       <c r="D412" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.3">
@@ -6392,7 +6392,7 @@
         <v>3</v>
       </c>
       <c r="D413" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.3">
@@ -6406,7 +6406,7 @@
         <v>3</v>
       </c>
       <c r="D414" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.3">
@@ -6434,7 +6434,7 @@
         <v>3</v>
       </c>
       <c r="D416" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.3">
@@ -6448,7 +6448,7 @@
         <v>3</v>
       </c>
       <c r="D417" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.3">
@@ -6462,7 +6462,7 @@
         <v>3</v>
       </c>
       <c r="D418" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.3">
@@ -6476,7 +6476,7 @@
         <v>3</v>
       </c>
       <c r="D419" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.3">
@@ -6686,7 +6686,7 @@
         <v>3</v>
       </c>
       <c r="D434" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.3">
@@ -6700,7 +6700,7 @@
         <v>3</v>
       </c>
       <c r="D435" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.3">
@@ -6770,7 +6770,7 @@
         <v>3</v>
       </c>
       <c r="D440" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.3">
@@ -6784,7 +6784,7 @@
         <v>3</v>
       </c>
       <c r="D441" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.3">
@@ -6854,7 +6854,7 @@
         <v>3</v>
       </c>
       <c r="D446" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.3">
@@ -6868,7 +6868,7 @@
         <v>3</v>
       </c>
       <c r="D447" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.3">
@@ -6882,7 +6882,7 @@
         <v>3</v>
       </c>
       <c r="D448" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.3">
@@ -6896,7 +6896,7 @@
         <v>3</v>
       </c>
       <c r="D449" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.3">
@@ -6910,7 +6910,7 @@
         <v>3</v>
       </c>
       <c r="D450" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.3">
@@ -6924,7 +6924,7 @@
         <v>3</v>
       </c>
       <c r="D451" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.3">
@@ -6952,7 +6952,7 @@
         <v>4</v>
       </c>
       <c r="D453" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.3">
@@ -6966,7 +6966,7 @@
         <v>4</v>
       </c>
       <c r="D454" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.3">
@@ -6980,7 +6980,7 @@
         <v>4</v>
       </c>
       <c r="D455" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.3">
@@ -6994,7 +6994,7 @@
         <v>4</v>
       </c>
       <c r="D456" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.3">
@@ -7008,7 +7008,7 @@
         <v>4</v>
       </c>
       <c r="D457" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.3">
@@ -7022,7 +7022,7 @@
         <v>4</v>
       </c>
       <c r="D458" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.3">
@@ -7036,7 +7036,7 @@
         <v>4</v>
       </c>
       <c r="D459" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.3">
@@ -7050,7 +7050,7 @@
         <v>4</v>
       </c>
       <c r="D460" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.3">
@@ -7064,7 +7064,7 @@
         <v>4</v>
       </c>
       <c r="D461" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.3">
@@ -7078,7 +7078,7 @@
         <v>4</v>
       </c>
       <c r="D462" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.3">
@@ -7092,7 +7092,7 @@
         <v>4</v>
       </c>
       <c r="D463" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.3">
@@ -7106,7 +7106,7 @@
         <v>4</v>
       </c>
       <c r="D464" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.3">
@@ -7120,7 +7120,7 @@
         <v>4</v>
       </c>
       <c r="D465" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.3">
@@ -7134,7 +7134,7 @@
         <v>4</v>
       </c>
       <c r="D466" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.3">
@@ -7148,7 +7148,7 @@
         <v>4</v>
       </c>
       <c r="D467" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.3">
@@ -7162,7 +7162,7 @@
         <v>4</v>
       </c>
       <c r="D468" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.3">
@@ -7176,7 +7176,7 @@
         <v>4</v>
       </c>
       <c r="D469" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.3">
@@ -7190,7 +7190,7 @@
         <v>4</v>
       </c>
       <c r="D470" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.3">
@@ -7204,7 +7204,7 @@
         <v>4</v>
       </c>
       <c r="D471" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.3">
@@ -7218,7 +7218,7 @@
         <v>4</v>
       </c>
       <c r="D472" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.3">
@@ -7232,7 +7232,7 @@
         <v>4</v>
       </c>
       <c r="D473" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.3">
@@ -7246,7 +7246,7 @@
         <v>4</v>
       </c>
       <c r="D474" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.3">
@@ -7260,7 +7260,7 @@
         <v>4</v>
       </c>
       <c r="D475" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.3">
@@ -7274,7 +7274,7 @@
         <v>4</v>
       </c>
       <c r="D476" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.3">
@@ -7288,7 +7288,7 @@
         <v>4</v>
       </c>
       <c r="D477" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.3">
@@ -7302,7 +7302,7 @@
         <v>4</v>
       </c>
       <c r="D478" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.3">
@@ -7316,7 +7316,7 @@
         <v>4</v>
       </c>
       <c r="D479" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.3">
@@ -7330,7 +7330,7 @@
         <v>4</v>
       </c>
       <c r="D480" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.3">
@@ -7344,7 +7344,7 @@
         <v>4</v>
       </c>
       <c r="D481" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.3">
@@ -7358,7 +7358,7 @@
         <v>4</v>
       </c>
       <c r="D482" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.3">
@@ -7372,7 +7372,7 @@
         <v>4</v>
       </c>
       <c r="D483" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.3">
@@ -7386,7 +7386,7 @@
         <v>4</v>
       </c>
       <c r="D484" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.3">
@@ -7400,7 +7400,7 @@
         <v>4</v>
       </c>
       <c r="D485" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.3">
@@ -7414,7 +7414,7 @@
         <v>4</v>
       </c>
       <c r="D486" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.3">
@@ -7428,7 +7428,7 @@
         <v>4</v>
       </c>
       <c r="D487" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.3">
@@ -7442,7 +7442,7 @@
         <v>4</v>
       </c>
       <c r="D488" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.3">
@@ -7456,7 +7456,7 @@
         <v>4</v>
       </c>
       <c r="D489" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.3">
@@ -7470,7 +7470,7 @@
         <v>4</v>
       </c>
       <c r="D490" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.3">
@@ -7484,7 +7484,7 @@
         <v>4</v>
       </c>
       <c r="D491" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.3">
@@ -7498,7 +7498,7 @@
         <v>4</v>
       </c>
       <c r="D492" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.3">
@@ -7512,7 +7512,7 @@
         <v>4</v>
       </c>
       <c r="D493" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.3">
@@ -7526,7 +7526,7 @@
         <v>4</v>
       </c>
       <c r="D494" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.3">
@@ -7540,7 +7540,7 @@
         <v>4</v>
       </c>
       <c r="D495" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.3">
@@ -7554,7 +7554,7 @@
         <v>4</v>
       </c>
       <c r="D496" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.3">
@@ -7568,7 +7568,7 @@
         <v>4</v>
       </c>
       <c r="D497" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.3">
@@ -7582,7 +7582,7 @@
         <v>4</v>
       </c>
       <c r="D498" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.3">
@@ -7596,7 +7596,7 @@
         <v>4</v>
       </c>
       <c r="D499" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.3">
@@ -7610,7 +7610,7 @@
         <v>4</v>
       </c>
       <c r="D500" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.3">
@@ -7624,7 +7624,7 @@
         <v>4</v>
       </c>
       <c r="D501" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.3">
@@ -7638,7 +7638,7 @@
         <v>4</v>
       </c>
       <c r="D502" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.3">
@@ -7652,7 +7652,7 @@
         <v>4</v>
       </c>
       <c r="D503" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.3">
@@ -7666,7 +7666,7 @@
         <v>4</v>
       </c>
       <c r="D504" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.3">
@@ -7680,7 +7680,7 @@
         <v>4</v>
       </c>
       <c r="D505" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.3">
@@ -7694,7 +7694,7 @@
         <v>4</v>
       </c>
       <c r="D506" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.3">
@@ -7708,7 +7708,7 @@
         <v>4</v>
       </c>
       <c r="D507" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.3">
@@ -7722,7 +7722,7 @@
         <v>4</v>
       </c>
       <c r="D508" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.3">
@@ -7736,7 +7736,7 @@
         <v>4</v>
       </c>
       <c r="D509" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.3">
@@ -8576,7 +8576,7 @@
         <v>3</v>
       </c>
       <c r="D569" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.3">
@@ -8590,7 +8590,7 @@
         <v>4</v>
       </c>
       <c r="D570" s="3" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>